<commit_message>
FAQ Automation Test DOne
</commit_message>
<xml_diff>
--- a/Test Cases and Reports/Automation Testing Reports/Test Case Report__Automation Testing.xlsx
+++ b/Test Cases and Reports/Automation Testing Reports/Test Case Report__Automation Testing.xlsx
@@ -8,15 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sheme\Downloads\Voice-Enabled-AI-Chatbot\Test Cases and Reports\Automation Testing Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84313802-F361-4173-A657-422D502979DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC6CD3E-A8CD-4F75-B7D7-EB79A4BEEA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{7F0DBCEC-97F8-4EA2-8E3E-675A0ECC9A2C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="4" xr2:uid="{7F0DBCEC-97F8-4EA2-8E3E-675A0ECC9A2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Role Page " sheetId="1" r:id="rId1"/>
     <sheet name="Student Page" sheetId="2" r:id="rId2"/>
     <sheet name="Instructor Page" sheetId="3" r:id="rId3"/>
     <sheet name="Admin Page" sheetId="4" r:id="rId4"/>
+    <sheet name="FAQ" sheetId="5" r:id="rId5"/>
+    <sheet name="Ask_Lumi Page" sheetId="6" r:id="rId6"/>
+    <sheet name="Setting Page" sheetId="8" r:id="rId7"/>
+    <sheet name="Voice Setting Page" sheetId="7" r:id="rId8"/>
+    <sheet name="Preferences_Setting Page" sheetId="9" r:id="rId9"/>
+    <sheet name="Notifications_Setting Page" sheetId="10" r:id="rId10"/>
+    <sheet name="Account_Setting Page" sheetId="11" r:id="rId11"/>
+    <sheet name="Reset_Password Page" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="229">
   <si>
     <t>Passed</t>
   </si>
@@ -609,6 +617,123 @@
   </si>
   <si>
     <t>TC_I123_Fail</t>
+  </si>
+  <si>
+    <t>Student Role Page Testing</t>
+  </si>
+  <si>
+    <t>Open Student Role Page</t>
+  </si>
+  <si>
+    <t>Page loads with title 'Student Role'</t>
+  </si>
+  <si>
+    <t>Page not loaded</t>
+  </si>
+  <si>
+    <t>Page failed to load initially</t>
+  </si>
+  <si>
+    <t>Page loaded successfully</t>
+  </si>
+  <si>
+    <t>Page loaded after fix</t>
+  </si>
+  <si>
+    <t>Locate Enrolled Courses Button</t>
+  </si>
+  <si>
+    <t>Button labeled 'Enrolled Courses' is visible</t>
+  </si>
+  <si>
+    <t>Button not visible</t>
+  </si>
+  <si>
+    <t>Button not visible due to CSS issue</t>
+  </si>
+  <si>
+    <t>Locate Upcoming Deadlines Button</t>
+  </si>
+  <si>
+    <t>Button labeled 'Upcoming Deadlines' is visible</t>
+  </si>
+  <si>
+    <t>Locate Submit Assignment Button</t>
+  </si>
+  <si>
+    <t>Button labeled 'Submit Assignment' is visible</t>
+  </si>
+  <si>
+    <t>Click Notifications Button</t>
+  </si>
+  <si>
+    <t>Button labeled 'Notifications' is visible</t>
+  </si>
+  <si>
+    <t>Button not displayed</t>
+  </si>
+  <si>
+    <t>Button did not trigger action</t>
+  </si>
+  <si>
+    <t>Button displayed</t>
+  </si>
+  <si>
+    <t>Button worked after fix</t>
+  </si>
+  <si>
+    <t>Click View Grades Button</t>
+  </si>
+  <si>
+    <t>Button labeled 'View Grades' is visible</t>
+  </si>
+  <si>
+    <t>Locate Logo</t>
+  </si>
+  <si>
+    <t>Logo not loaded</t>
+  </si>
+  <si>
+    <t>Logo not loaded due to incorrect src</t>
+  </si>
+  <si>
+    <t>Locate Footer Section</t>
+  </si>
+  <si>
+    <t>Footer loaded correctly</t>
+  </si>
+  <si>
+    <t>Help page displayed</t>
+  </si>
+  <si>
+    <t>Help page displayed correctly</t>
+  </si>
+  <si>
+    <t>FAQ page displayed</t>
+  </si>
+  <si>
+    <t>FAQ page displayed correctly</t>
+  </si>
+  <si>
+    <t>Contact Us page displayed</t>
+  </si>
+  <si>
+    <t>Contact Us page displayed correctly</t>
+  </si>
+  <si>
+    <t>Student Role Navigation</t>
+  </si>
+  <si>
+    <t>Student page loaded</t>
+  </si>
+  <si>
+    <t>Navigation successful</t>
+  </si>
+  <si>
+    <t>Admin page loaded</t>
+  </si>
+  <si>
+    <t>Instructor page loaded</t>
   </si>
 </sst>
 </file>
@@ -637,7 +762,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -647,6 +772,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -678,7 +809,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -686,6 +817,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1025,7 +1159,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1423,16 +1557,510 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2424F36-BCEE-41D3-AC37-F749302BFA43}">
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26451393-9676-4489-9962-99266338B49A}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5FC781-E6AB-4045-855A-74CA3513D647}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76C5A1BD-6D63-4392-999B-551C7AACA2A7}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2424F36-BCEE-41D3-AC37-F749302BFA43}">
+  <dimension ref="A1:H17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="32.21875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="43.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.5546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.77734375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="35.5546875" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2683,4 +3311,72 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B49A81D8-CC9F-4BA4-ACD5-8B1BDA7C4E73}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7245FF9C-FCAE-4C5E-A62F-2E7112D85630}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86887CBF-B4C2-4145-845B-97087FA2760D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9389862-AC8B-4BF0-8120-DBA02EFC90D1}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O31" sqref="O31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EAD83A1-D776-4E67-9D19-4495B18746FF}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>